<commit_message>
All functions tested and working
also had to do a bit of tidying up in the GUI
</commit_message>
<xml_diff>
--- a/TableFormat_TestPrograms.xlsx
+++ b/TableFormat_TestPrograms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patog\WorkFolders\Eclipse\GitWorkspace\esolang_tableformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405A8A55-8E85-496F-8C2F-2F84B7DE519F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90319A8-E988-4789-A850-93EC1904FAE4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="2" xr2:uid="{C5F2AF3F-BC32-4708-84D4-A5AEDD116D48}"/>
   </bookViews>
@@ -17,10 +17,15 @@
     <sheet name="helloWorld" sheetId="2" r:id="rId2"/>
     <sheet name="functionsTest" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -390,7 +395,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,8 +435,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF55FFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="25">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,12 +537,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF000055"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -573,6 +580,126 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00AAFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF550000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5500FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF555500"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF555555"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5555AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5555FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55AA00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55AA55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55AAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55AAFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55FF55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55FFAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAA00AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAA00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -607,8 +734,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
@@ -616,7 +742,31 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -625,16 +775,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF00AAFF"/>
-      <color rgb="FF550055"/>
-      <color rgb="FF00AAAA"/>
-      <color rgb="FF0055FF"/>
-      <color rgb="FF0055AA"/>
-      <color rgb="FF005500"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF55FFFF"/>
+      <color rgb="FF550000"/>
       <color rgb="FF000055"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFAA5555"/>
       <color rgb="FFAA5500"/>
+      <color rgb="FFAA00FF"/>
+      <color rgb="FFAA00AA"/>
+      <color rgb="FFAA0055"/>
+      <color rgb="FFAA0000"/>
+      <color rgb="FF55FFAA"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1323,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DECA280-14F4-4BCB-ADF9-F5DE8F3639BE}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1486,10 @@
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="Z1">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="AB1" t="s">
@@ -1347,6 +1500,9 @@
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
       <c r="AA2" s="6" t="s">
         <v>17</v>
       </c>
@@ -1361,10 +1517,13 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="AA3" s="20" t="s">
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="18" t="s">
         <v>18</v>
       </c>
       <c r="AB3" t="s">
@@ -1375,13 +1534,16 @@
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AA4" s="21" t="s">
+      <c r="Z4">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="19" t="s">
         <v>19</v>
       </c>
       <c r="AB4" t="s">
@@ -1389,14 +1551,17 @@
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>61</v>
+      </c>
+      <c r="Z5">
+        <v>5</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>20</v>
@@ -1406,10 +1571,13 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="AA6" s="22" t="s">
+      <c r="Z6">
+        <v>6</v>
+      </c>
+      <c r="AA6" s="20" t="s">
         <v>21</v>
       </c>
       <c r="AB6" t="s">
@@ -1420,7 +1588,10 @@
       <c r="B7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AA7" s="23" t="s">
+      <c r="Z7">
+        <v>7</v>
+      </c>
+      <c r="AA7" s="21" t="s">
         <v>22</v>
       </c>
       <c r="AB7" t="s">
@@ -1428,11 +1599,14 @@
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
+      <c r="Z8">
+        <v>8</v>
+      </c>
       <c r="AA8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1444,6 +1618,9 @@
       <c r="B9" s="7" t="s">
         <v>69</v>
       </c>
+      <c r="Z9">
+        <v>9</v>
+      </c>
       <c r="AA9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1455,7 +1632,10 @@
       <c r="B10" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA10" s="24" t="s">
+      <c r="Z10">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="22" t="s">
         <v>25</v>
       </c>
       <c r="AB10" t="s">
@@ -1463,10 +1643,13 @@
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="24">
+      <c r="B11" s="22">
         <v>10</v>
       </c>
-      <c r="AA11" s="26" t="s">
+      <c r="Z11">
+        <v>11</v>
+      </c>
+      <c r="AA11" s="24" t="s">
         <v>26</v>
       </c>
       <c r="AB11" t="s">
@@ -1474,16 +1657,16 @@
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>59</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -1492,7 +1675,7 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="47" t="s">
         <v>51</v>
       </c>
       <c r="I12" s="4" t="s">
@@ -1501,13 +1684,16 @@
       <c r="J12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="17">
         <v>1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="Z12">
+        <v>12</v>
+      </c>
+      <c r="AA12" s="27" t="s">
         <v>27</v>
       </c>
       <c r="AB12" t="s">
@@ -1530,7 +1716,10 @@
       <c r="L13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="Z13">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="29" t="s">
         <v>28</v>
       </c>
       <c r="AB13" t="s">
@@ -1541,19 +1730,22 @@
       <c r="B14" s="1">
         <v>1234</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="17">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="Z14">
+        <v>14</v>
+      </c>
+      <c r="AA14" s="28" t="s">
         <v>29</v>
       </c>
       <c r="AB14" t="s">
@@ -1561,13 +1753,13 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="32" t="s">
         <v>100</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1576,7 +1768,10 @@
       <c r="L15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="Z15">
+        <v>15</v>
+      </c>
+      <c r="AA15" s="30" t="s">
         <v>30</v>
       </c>
       <c r="AB15" t="s">
@@ -1584,7 +1779,7 @@
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1593,13 +1788,16 @@
       <c r="D16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="39" t="s">
         <v>111</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="Z16">
+        <v>16</v>
+      </c>
+      <c r="AA16" s="31" t="s">
         <v>31</v>
       </c>
       <c r="AB16" t="s">
@@ -1610,19 +1808,22 @@
       <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>2</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="AA17" s="25" t="s">
+      <c r="Z17">
+        <v>17</v>
+      </c>
+      <c r="AA17" s="23" t="s">
         <v>32</v>
       </c>
       <c r="AB17" t="s">
@@ -1630,22 +1831,25 @@
       </c>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="Z18">
+        <v>18</v>
+      </c>
+      <c r="AA18" s="26" t="s">
         <v>33</v>
       </c>
       <c r="AB18" t="s">
@@ -1656,20 +1860,23 @@
       <c r="B19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="28" t="s">
         <v>82</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="31" t="s">
         <v>89</v>
       </c>
       <c r="Q19" s="2"/>
-      <c r="AA19" t="s">
+      <c r="Z19">
+        <v>19</v>
+      </c>
+      <c r="AA19" s="32" t="s">
         <v>34</v>
       </c>
       <c r="AB19" t="s">
@@ -1677,19 +1884,19 @@
       </c>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="3">
+        <v>5</v>
+      </c>
+      <c r="D20" s="18">
         <v>3</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="18">
         <v>3</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="47" t="s">
         <v>51</v>
       </c>
       <c r="M20" s="4" t="s">
@@ -1698,16 +1905,19 @@
       <c r="N20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="O20" s="17">
+      <c r="O20" s="49">
         <v>2000</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="48" t="s">
         <v>52</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="Z20">
+        <v>20</v>
+      </c>
+      <c r="AA20" s="33" t="s">
         <v>35</v>
       </c>
       <c r="AB20" t="s">
@@ -1715,19 +1925,22 @@
       </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="28" t="s">
         <v>82</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="32" t="s">
         <v>100</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="Z21">
+        <v>21</v>
+      </c>
+      <c r="AA21" s="34" t="s">
         <v>36</v>
       </c>
       <c r="AB21" t="s">
@@ -1735,19 +1948,22 @@
       </c>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="Z22">
+        <v>22</v>
+      </c>
+      <c r="AA22" s="35" t="s">
         <v>37</v>
       </c>
       <c r="AB22" t="s">
@@ -1755,19 +1971,22 @@
       </c>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="29">
         <v>13</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>2</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="Z23">
+        <v>23</v>
+      </c>
+      <c r="AA23" s="36" t="s">
         <v>38</v>
       </c>
       <c r="AB23" t="s">
@@ -1781,13 +2000,16 @@
       <c r="C24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="33" t="s">
         <v>101</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="Z24">
+        <v>24</v>
+      </c>
+      <c r="AA24" s="37" t="s">
         <v>39</v>
       </c>
       <c r="AB24" t="s">
@@ -1795,7 +2017,7 @@
       </c>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1804,10 +2026,13 @@
       <c r="D25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="Z25">
+        <v>25</v>
+      </c>
+      <c r="AA25" s="38" t="s">
         <v>40</v>
       </c>
       <c r="AB25" t="s">
@@ -1815,19 +2040,22 @@
       </c>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="17">
         <v>1</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="Z26">
+        <v>26</v>
+      </c>
+      <c r="AA26" s="39" t="s">
         <v>41</v>
       </c>
       <c r="AB26" t="s">
@@ -1838,7 +2066,7 @@
       <c r="B27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -1847,7 +2075,10 @@
       <c r="E27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="Z27">
+        <v>27</v>
+      </c>
+      <c r="AA27" s="40" t="s">
         <v>42</v>
       </c>
       <c r="AB27" t="s">
@@ -1855,7 +2086,7 @@
       </c>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="40" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1867,7 +2098,10 @@
       <c r="E28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="Z28">
+        <v>28</v>
+      </c>
+      <c r="AA28" s="41" t="s">
         <v>43</v>
       </c>
       <c r="AB28" t="s">
@@ -1875,19 +2109,22 @@
       </c>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="17">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="Z29">
+        <v>29</v>
+      </c>
+      <c r="AA29" s="42" t="s">
         <v>44</v>
       </c>
       <c r="AB29" t="s">
@@ -1898,16 +2135,19 @@
       <c r="B30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="34" t="s">
         <v>104</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="Z30">
+        <v>30</v>
+      </c>
+      <c r="AA30" s="43" t="s">
         <v>45</v>
       </c>
       <c r="AB30" t="s">
@@ -1915,7 +2155,7 @@
       </c>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="41" t="s">
         <v>43</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1924,10 +2164,13 @@
       <c r="D31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="Z31">
+        <v>31</v>
+      </c>
+      <c r="AA31" s="44" t="s">
         <v>46</v>
       </c>
       <c r="AB31" t="s">
@@ -1935,19 +2178,22 @@
       </c>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B32" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>2</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="Z32">
+        <v>32</v>
+      </c>
+      <c r="AA32" s="12" t="s">
         <v>47</v>
       </c>
       <c r="AB32" t="s">
@@ -1958,16 +2204,19 @@
       <c r="B33" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="AA33" t="s">
+      <c r="Z33">
+        <v>33</v>
+      </c>
+      <c r="AA33" s="13" t="s">
         <v>48</v>
       </c>
       <c r="AB33" t="s">
@@ -1975,7 +2224,7 @@
       </c>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="B34" s="42" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1984,10 +2233,13 @@
       <c r="D34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="Z34">
+        <v>34</v>
+      </c>
+      <c r="AA34" s="45" t="s">
         <v>49</v>
       </c>
       <c r="AB34" t="s">
@@ -1995,19 +2247,22 @@
       </c>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="B35" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="18">
         <v>3</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="18">
         <v>3</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="Z35">
+        <v>35</v>
+      </c>
+      <c r="AA35" s="46" t="s">
         <v>50</v>
       </c>
       <c r="AB35" t="s">
@@ -2018,16 +2273,19 @@
       <c r="B36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="34" t="s">
         <v>104</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="Z36">
+        <v>36</v>
+      </c>
+      <c r="AA36" s="47" t="s">
         <v>51</v>
       </c>
       <c r="AB36" t="s">
@@ -2035,19 +2293,22 @@
       </c>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="Z37">
+        <v>37</v>
+      </c>
+      <c r="AA37" s="48" t="s">
         <v>52</v>
       </c>
       <c r="AB37" t="s">
@@ -2058,8 +2319,11 @@
       <c r="D38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="6">
         <v>2</v>
+      </c>
+      <c r="Z38">
+        <v>38</v>
       </c>
       <c r="AA38" s="5" t="s">
         <v>53</v>
@@ -2069,13 +2333,13 @@
       </c>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+      <c r="D39" s="35" t="s">
         <v>105</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA39" s="18" t="s">
+      <c r="AA39" s="25" t="s">
         <v>54</v>
       </c>
       <c r="AB39" t="s">
@@ -2086,15 +2350,15 @@
       <c r="D40" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="36" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="41" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
+      <c r="D41" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2107,10 +2371,10 @@
       </c>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="17" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Work on first actual program
It's gonna be a sort
</commit_message>
<xml_diff>
--- a/TableFormat_TestPrograms.xlsx
+++ b/TableFormat_TestPrograms.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patog\WorkFolders\Eclipse\GitWorkspace\esolang_tableformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90319A8-E988-4789-A850-93EC1904FAE4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E0D7A9-6172-4D08-B420-4CB6965AF925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="2" xr2:uid="{C5F2AF3F-BC32-4708-84D4-A5AEDD116D48}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="3" xr2:uid="{C5F2AF3F-BC32-4708-84D4-A5AEDD116D48}"/>
   </bookViews>
   <sheets>
     <sheet name="firstTest" sheetId="1" r:id="rId1"/>
     <sheet name="helloWorld" sheetId="2" r:id="rId2"/>
     <sheet name="functionsTest" sheetId="3" r:id="rId3"/>
+    <sheet name="sort" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="147">
   <si>
     <t>nextAsNumber</t>
   </si>
@@ -389,6 +390,90 @@
   </si>
   <si>
     <t>q20</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>printchar</t>
+  </si>
+  <si>
+    <t>F[0]</t>
+  </si>
+  <si>
+    <t>number of elements</t>
+  </si>
+  <si>
+    <t>F[1]</t>
+  </si>
+  <si>
+    <t>F[2]</t>
+  </si>
+  <si>
+    <t>F[3]</t>
+  </si>
+  <si>
+    <t>F[4]</t>
+  </si>
+  <si>
+    <t>F[5]</t>
+  </si>
+  <si>
+    <t>F[6]</t>
+  </si>
+  <si>
+    <t>F[7]</t>
+  </si>
+  <si>
+    <t>loading cycle variable</t>
+  </si>
+  <si>
+    <t>outer sort cycle variable</t>
+  </si>
+  <si>
+    <t>inner sort cycle variable</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>&lt;loop end&gt;</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>the array</t>
+  </si>
+  <si>
+    <t>&lt;first test end&gt;</t>
   </si>
 </sst>
 </file>
@@ -1473,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DECA280-14F4-4BCB-ADF9-F5DE8F3639BE}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA38" sqref="AA1:AA38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,4 +2467,677 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B36A6A3-FA3E-45F9-8203-DB8FCE0044E6}">
+  <dimension ref="A1:AB57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="26" max="26" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z11" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z12" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z13" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z14" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z15" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z16" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z17" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z18" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z19" s="32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z20" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z21" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z22" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z23" s="36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z24" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z25" s="38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z26" s="39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z27" s="40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z28" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z29" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z30" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z31" s="44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z32" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z33" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z34" s="45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z35" s="46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z36" s="47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z37" s="48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z38" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more debug help
also made my first-ever loop work
</commit_message>
<xml_diff>
--- a/TableFormat_TestPrograms.xlsx
+++ b/TableFormat_TestPrograms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patog\WorkFolders\Eclipse\GitWorkspace\esolang_tableformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E0D7A9-6172-4D08-B420-4CB6965AF925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A86338A-D9D0-4101-8ADD-8F0B1BE2778D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="3" xr2:uid="{C5F2AF3F-BC32-4708-84D4-A5AEDD116D48}"/>
   </bookViews>
@@ -529,7 +529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="53">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,6 +785,60 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAA00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAAFF55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAAFFAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5555"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5500"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAAAA00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -852,6 +906,17 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="5" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -860,16 +925,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF55FFFF"/>
-      <color rgb="FF550000"/>
+      <color rgb="FFAA5555"/>
+      <color rgb="FFAAAA00"/>
+      <color rgb="FFFF5500"/>
+      <color rgb="FFFF5555"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFAAFFAA"/>
+      <color rgb="FF00AA55"/>
       <color rgb="FF000055"/>
-      <color rgb="FFAA5555"/>
-      <color rgb="FFAA5500"/>
-      <color rgb="FFAA00FF"/>
-      <color rgb="FFAA00AA"/>
-      <color rgb="FFAA0055"/>
-      <color rgb="FFAA0000"/>
-      <color rgb="FF55FFAA"/>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF00FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1559,7 +1624,7 @@
   <dimension ref="A1:AB43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA38" sqref="AA1:AA38"/>
+      <selection activeCell="Z1" sqref="Z1:Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2474,7 +2539,7 @@
   <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,7 +2577,7 @@
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="Z3" s="18" t="s">
@@ -2551,7 +2616,7 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="Z6" s="20" t="s">
@@ -2584,7 +2649,7 @@
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
       <c r="Z9" s="7" t="s">
@@ -2601,7 +2666,7 @@
       <c r="A10" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="Z10" s="22" t="s">
@@ -2620,7 +2685,7 @@
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K12" t="s">
@@ -2634,7 +2699,7 @@
       <c r="A13" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="19" t="s">
         <v>59</v>
       </c>
       <c r="K13" s="17" t="s">
@@ -2648,31 +2713,31 @@
       <c r="A14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="19" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="17">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="19" t="s">
         <v>59</v>
       </c>
       <c r="I14" t="s">
         <v>54</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="47" t="s">
         <v>51</v>
       </c>
       <c r="K14" s="17" t="s">
@@ -2683,7 +2748,7 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="50" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2703,13 +2768,13 @@
       <c r="A16" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="55" t="s">
         <v>124</v>
       </c>
       <c r="H16" t="s">
         <v>54</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="32" t="s">
         <v>100</v>
       </c>
       <c r="Z16" s="31" t="s">
@@ -2726,7 +2791,7 @@
       <c r="H17" t="s">
         <v>54</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="12" t="s">
         <v>47</v>
       </c>
       <c r="Z17" s="23" t="s">
@@ -2734,7 +2799,7 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="51" t="s">
         <v>120</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -2743,7 +2808,7 @@
       <c r="H18" t="s">
         <v>54</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="31" t="s">
         <v>89</v>
       </c>
       <c r="Z18" s="26" t="s">
@@ -2754,13 +2819,13 @@
       <c r="A19" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="50" t="s">
         <v>119</v>
       </c>
       <c r="H19" t="s">
         <v>54</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="23" t="s">
         <v>75</v>
       </c>
       <c r="Z19" s="32" t="s">
@@ -2777,8 +2842,8 @@
       <c r="H20" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="I20" t="s">
-        <v>54</v>
+      <c r="I20" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="J20" s="18" t="s">
         <v>63</v>
@@ -2788,7 +2853,7 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="52" t="s">
         <v>121</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2802,7 +2867,7 @@
       <c r="A22" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="54" t="s">
         <v>123</v>
       </c>
       <c r="Z22" s="35" t="s">
@@ -2821,7 +2886,7 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="53" t="s">
         <v>122</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -2835,7 +2900,7 @@
       <c r="A25" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="52" t="s">
         <v>121</v>
       </c>
       <c r="Z25" s="38" t="s">
@@ -2854,7 +2919,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2868,7 +2933,7 @@
       <c r="A28" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="12" t="s">
         <v>11</v>
       </c>
       <c r="Z28" s="41" t="s">
@@ -2887,7 +2952,7 @@
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="52" t="s">
         <v>121</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -2901,7 +2966,7 @@
       <c r="A31" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="9" t="s">
         <v>8</v>
       </c>
       <c r="Z31" s="44" t="s">
@@ -2920,7 +2985,7 @@
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="54" t="s">
         <v>123</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -2934,7 +2999,7 @@
       <c r="A34" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="60" t="s">
         <v>142</v>
       </c>
       <c r="Z34" s="45" t="s">
@@ -2953,7 +3018,7 @@
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="50" t="s">
         <v>119</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -2967,7 +3032,7 @@
       <c r="A37" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="59" t="s">
         <v>140</v>
       </c>
       <c r="Z37" s="48" t="s">
@@ -2986,7 +3051,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="55" t="s">
         <v>124</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -2997,7 +3062,7 @@
       <c r="A40" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3010,7 +3075,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="56" t="s">
         <v>125</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -3021,7 +3086,7 @@
       <c r="A43" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="59" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3034,7 +3099,7 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -3042,10 +3107,10 @@
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="54" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3058,7 +3123,7 @@
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="17">
         <v>1</v>
       </c>
       <c r="B48" s="7" t="s">
@@ -3066,15 +3131,15 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="58" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="29" t="s">
         <v>85</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -3082,7 +3147,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -3093,12 +3158,12 @@
       <c r="A52" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="52" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="6">
         <v>2</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -3106,7 +3171,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="22" t="s">
         <v>73</v>
       </c>
       <c r="B54" s="7" t="s">
@@ -3114,15 +3179,15 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="57" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3130,7 +3195,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -3139,5 +3204,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proof text don't matter
made a copy of sort and replaced the text with the Wikipedia article on Bubblesort
</commit_message>
<xml_diff>
--- a/TableFormat_TestPrograms.xlsx
+++ b/TableFormat_TestPrograms.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patog\WorkFolders\Eclipse\GitWorkspace\esolang_tableformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830FADB7-851E-45D4-80F8-3098E375BFEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82375751-16A7-4A64-A259-96DE83F55D2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="3" xr2:uid="{C5F2AF3F-BC32-4708-84D4-A5AEDD116D48}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="4" xr2:uid="{C5F2AF3F-BC32-4708-84D4-A5AEDD116D48}"/>
   </bookViews>
   <sheets>
     <sheet name="firstTest" sheetId="1" r:id="rId1"/>
     <sheet name="helloWorld" sheetId="2" r:id="rId2"/>
     <sheet name="functionsTest" sheetId="3" r:id="rId3"/>
     <sheet name="sort" sheetId="4" r:id="rId4"/>
+    <sheet name="sortButRandomText" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="307">
   <si>
     <t>nextAsNumber</t>
   </si>
@@ -477,13 +478,490 @@
   </si>
   <si>
     <t>print cycle variable</t>
+  </si>
+  <si>
+    <t>Bubble</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>sometimes</t>
+  </si>
+  <si>
+    <t>reffered</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>sinking</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>sorting</t>
+  </si>
+  <si>
+    <t>algorithm</t>
+  </si>
+  <si>
+    <t>that</t>
+  </si>
+  <si>
+    <t>repeatedly</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>through</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>sorted</t>
+  </si>
+  <si>
+    <t>compares</t>
+  </si>
+  <si>
+    <t>each</t>
+  </si>
+  <si>
+    <t>pair</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>adjacent</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>swaps</t>
+  </si>
+  <si>
+    <t>them</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>they</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>repeated</t>
+  </si>
+  <si>
+    <t>until</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>which</t>
+  </si>
+  <si>
+    <t>indicates</t>
+  </si>
+  <si>
+    <t>comparison</t>
+  </si>
+  <si>
+    <t>named</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>way</t>
+  </si>
+  <si>
+    <t>smaller</t>
+  </si>
+  <si>
+    <t>larger</t>
+  </si>
+  <si>
+    <t>elements</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>bubble</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>Although</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>too</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>impractical</t>
+  </si>
+  <si>
+    <t>most</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>even</t>
+  </si>
+  <si>
+    <t>when</t>
+  </si>
+  <si>
+    <t>compared</t>
+  </si>
+  <si>
+    <t>insertion</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>practical</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>mostly</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>out-of-order</t>
+  </si>
+  <si>
+    <t>nearly</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>performance</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>worst-case</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>complexity</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>n^2</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>being</t>
+  </si>
+  <si>
+    <t>Most</t>
+  </si>
+  <si>
+    <t>algorithms</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>substantially</t>
+  </si>
+  <si>
+    <t>better</t>
+  </si>
+  <si>
+    <t>often</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>Even</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>such</t>
+  </si>
+  <si>
+    <t>generally</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>faster</t>
+  </si>
+  <si>
+    <t>than</t>
+  </si>
+  <si>
+    <t>more</t>
+  </si>
+  <si>
+    <t>complex</t>
+  </si>
+  <si>
+    <t>Therefore</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>only</t>
+  </si>
+  <si>
+    <t>significant</t>
+  </si>
+  <si>
+    <t>advantage</t>
+  </si>
+  <si>
+    <t>over</t>
+  </si>
+  <si>
+    <t>quicksort</t>
+  </si>
+  <si>
+    <t>but</t>
+  </si>
+  <si>
+    <t>ability</t>
+  </si>
+  <si>
+    <t>detect</t>
+  </si>
+  <si>
+    <t>efficiently</t>
+  </si>
+  <si>
+    <t>built</t>
+  </si>
+  <si>
+    <t>into</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>already</t>
+  </si>
+  <si>
+    <t>best-case</t>
+  </si>
+  <si>
+    <t>By</t>
+  </si>
+  <si>
+    <t>contrast</t>
+  </si>
+  <si>
+    <t>those</t>
+  </si>
+  <si>
+    <t>average-case</t>
+  </si>
+  <si>
+    <t>perform</t>
+  </si>
+  <si>
+    <t>their</t>
+  </si>
+  <si>
+    <t>entire</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>thus</t>
+  </si>
+  <si>
+    <t>However</t>
+  </si>
+  <si>
+    <t>does</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>also</t>
+  </si>
+  <si>
+    <t>performs</t>
+  </si>
+  <si>
+    <t>sortd</t>
+  </si>
+  <si>
+    <t>having</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>inversions</t>
+  </si>
+  <si>
+    <t>should</t>
+  </si>
+  <si>
+    <t>avoided</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>collections</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>will</t>
+  </si>
+  <si>
+    <t>efficient</t>
+  </si>
+  <si>
+    <t>reverse-ordered</t>
+  </si>
+  <si>
+    <t>collection</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>must</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>during</t>
+  </si>
+  <si>
+    <t>determines</t>
+  </si>
+  <si>
+    <t>sort's</t>
+  </si>
+  <si>
+    <t>because</t>
+  </si>
+  <si>
+    <t>different</t>
+  </si>
+  <si>
+    <t>directions</t>
+  </si>
+  <si>
+    <t>at</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +1004,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF55FFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -858,7 +1345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -920,6 +1407,9 @@
     <xf numFmtId="0" fontId="3" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -2541,8 +3031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B36A6A3-FA3E-45F9-8203-DB8FCE0044E6}">
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G38" sqref="A1:T57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,4 +4500,1280 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB87F3F-8A90-4E5B-9D50-CA181F7F3E9B}">
+  <dimension ref="A1:U57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="U1" s="61"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>174</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="S5" s="27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" t="s">
+        <v>180</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="S6" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="S7" s="22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I8" t="s">
+        <v>174</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="M8" t="s">
+        <v>188</v>
+      </c>
+      <c r="S8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="I9" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="M9" t="s">
+        <v>165</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="M10" t="s">
+        <v>189</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="S10" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="K11" t="s">
+        <v>195</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="R11" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="S11" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M12" t="s">
+        <v>164</v>
+      </c>
+      <c r="R12" s="27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="M13" t="s">
+        <v>159</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="I14" t="s">
+        <v>193</v>
+      </c>
+      <c r="J14" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="M14" t="s">
+        <v>208</v>
+      </c>
+      <c r="R14" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H15" t="s">
+        <v>211</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="M15" t="s">
+        <v>182</v>
+      </c>
+      <c r="R15" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="H16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="M16" t="s">
+        <v>176</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H17" t="s">
+        <v>179</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="M17" t="s">
+        <v>167</v>
+      </c>
+      <c r="R17" s="31" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="H18" t="s">
+        <v>218</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="M18" t="s">
+        <v>219</v>
+      </c>
+      <c r="R18" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="H19" t="s">
+        <v>221</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="M19" t="s">
+        <v>149</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="N20" t="s">
+        <v>227</v>
+      </c>
+      <c r="O20" t="s">
+        <v>228</v>
+      </c>
+      <c r="P20" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>230</v>
+      </c>
+      <c r="R20" t="s">
+        <v>150</v>
+      </c>
+      <c r="S20" t="s">
+        <v>231</v>
+      </c>
+      <c r="T20" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="R21" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="T21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>233</v>
+      </c>
+      <c r="R22" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="T22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="R23" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="T23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="53" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="T24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="R25" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="T25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="R26" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="T26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="R27" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="T27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="R28" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="T28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="T29" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="R30" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="T30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="R31" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="T31" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="R32" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="T32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="R33" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="T33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B34" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="G34" t="s">
+        <v>250</v>
+      </c>
+      <c r="H34" t="s">
+        <v>150</v>
+      </c>
+      <c r="I34" t="s">
+        <v>199</v>
+      </c>
+      <c r="J34" t="s">
+        <v>149</v>
+      </c>
+      <c r="K34" t="s">
+        <v>156</v>
+      </c>
+      <c r="L34" t="s">
+        <v>251</v>
+      </c>
+      <c r="M34" t="s">
+        <v>120</v>
+      </c>
+      <c r="N34" t="s">
+        <v>213</v>
+      </c>
+      <c r="O34" t="s">
+        <v>158</v>
+      </c>
+      <c r="P34" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>182</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="T34" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F35" t="s">
+        <v>160</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="T35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F36" t="s">
+        <v>206</v>
+      </c>
+      <c r="R36" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="T36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="F37" t="s">
+        <v>256</v>
+      </c>
+      <c r="R37" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="T37" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F38" t="s">
+        <v>149</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="T38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="G39" t="s">
+        <v>153</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="R39" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="T39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F40" t="s">
+        <v>164</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="M40" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="N40" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="R40" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="T40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F41" t="s">
+        <v>167</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="M41" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="N41" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="R41" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="T41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F42" t="s">
+        <v>199</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R42" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="T42" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="F43" t="s">
+        <v>230</v>
+      </c>
+      <c r="L43" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="N43" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="R43" t="s">
+        <v>267</v>
+      </c>
+      <c r="T43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F44" t="s">
+        <v>235</v>
+      </c>
+      <c r="L44" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="N44" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="R44" t="s">
+        <v>268</v>
+      </c>
+      <c r="T44" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F45" t="s">
+        <v>226</v>
+      </c>
+      <c r="L45" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="N45" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="R45" t="s">
+        <v>271</v>
+      </c>
+      <c r="T45" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" s="54" t="s">
+        <v>273</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G46" t="s">
+        <v>164</v>
+      </c>
+      <c r="H46" t="s">
+        <v>275</v>
+      </c>
+      <c r="I46" t="s">
+        <v>43</v>
+      </c>
+      <c r="J46" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="L46" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="N46" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="R46" t="s">
+        <v>249</v>
+      </c>
+      <c r="T46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F47" t="s">
+        <v>251</v>
+      </c>
+      <c r="J47" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="R47" t="s">
+        <v>149</v>
+      </c>
+      <c r="T47" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="F48" t="s">
+        <v>150</v>
+      </c>
+      <c r="J48" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="N48" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="R48" t="s">
+        <v>282</v>
+      </c>
+      <c r="T48" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="B49" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" t="s">
+        <v>165</v>
+      </c>
+      <c r="J49" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="L49" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="N49" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="R49" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="S49" t="s">
+        <v>284</v>
+      </c>
+      <c r="T49" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F50" t="s">
+        <v>171</v>
+      </c>
+      <c r="J50" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="L50" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="N50" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q50" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="R50" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="S50" t="s">
+        <v>287</v>
+      </c>
+      <c r="T50" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F51" t="s">
+        <v>164</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L51" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="N51" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q51" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" s="52" t="s">
+        <v>292</v>
+      </c>
+      <c r="F52" t="s">
+        <v>293</v>
+      </c>
+      <c r="J52" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="K52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L52" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q52" s="31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F53" t="s">
+        <v>295</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q53" s="23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G54" t="s">
+        <v>197</v>
+      </c>
+      <c r="H54" t="s">
+        <v>298</v>
+      </c>
+      <c r="I54" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="J54" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="K54" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="L54" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="N54" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="O54" t="s">
+        <v>302</v>
+      </c>
+      <c r="P54" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q54" s="18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" s="57" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Just made columns right size
</commit_message>
<xml_diff>
--- a/TableFormat_TestPrograms.xlsx
+++ b/TableFormat_TestPrograms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patog\WorkFolders\Eclipse\GitWorkspace\esolang_tableformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82375751-16A7-4A64-A259-96DE83F55D2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028EBE8C-F06C-4D86-9C61-D5A9B4372014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="4" xr2:uid="{C5F2AF3F-BC32-4708-84D4-A5AEDD116D48}"/>
   </bookViews>
@@ -4506,11 +4506,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB87F3F-8A90-4E5B-9D50-CA181F7F3E9B}">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">

</xml_diff>